<commit_message>
H2 Database set up
</commit_message>
<xml_diff>
--- a/src/main/resources/hr-leaseplan.xlsx
+++ b/src/main/resources/hr-leaseplan.xlsx
@@ -8,36 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eclipse-workspace\hr-leaseplan-project\hr-leaseplan-project\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDF378A-4154-457C-8D9F-5468ECF37146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE28BC5-054A-478F-A46E-155CCDB4CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7F8BE8A6-5FEF-41F6-9968-76C7035C40E5}"/>
+    <workbookView xWindow="-28920" yWindow="3720" windowWidth="29040" windowHeight="15840" xr2:uid="{7F8BE8A6-5FEF-41F6-9968-76C7035C40E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Employee Number</t>
   </si>
@@ -117,15 +105,9 @@
     <t>1.5 TSI HIGHLINE OPF</t>
   </si>
   <si>
-    <t>575.00</t>
-  </si>
-  <si>
     <t>LPB</t>
   </si>
   <si>
-    <t>75.00</t>
-  </si>
-  <si>
     <t>Smith, John</t>
   </si>
   <si>
@@ -187,39 +169,12 @@
   </si>
   <si>
     <t>A 160 CDI</t>
-  </si>
-  <si>
-    <t>575.01</t>
-  </si>
-  <si>
-    <t>575.02</t>
-  </si>
-  <si>
-    <t>575.03</t>
-  </si>
-  <si>
-    <t>575.04</t>
-  </si>
-  <si>
-    <t>75.01</t>
-  </si>
-  <si>
-    <t>75.02</t>
-  </si>
-  <si>
-    <t>75.03</t>
-  </si>
-  <si>
-    <t>75.04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,12 +239,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -607,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418E76DB-9A9E-421F-B9A7-2282E37ED3C7}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +572,7 @@
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -702,13 +658,13 @@
         <v>53331</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4">
-        <v>37.091999999999999</v>
+      <c r="D2" s="3">
+        <v>37092</v>
       </c>
       <c r="E2">
         <v>122</v>
@@ -746,17 +702,17 @@
       <c r="P2" s="2">
         <v>46262</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="4">
+        <v>575</v>
+      </c>
+      <c r="R2" t="s">
         <v>26</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
       </c>
       <c r="S2" s="2">
         <v>44811</v>
       </c>
-      <c r="T2" t="s">
-        <v>28</v>
+      <c r="T2" s="5">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -764,13 +720,13 @@
         <v>169953</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="4">
-        <v>39.769276958773091</v>
+        <v>32</v>
+      </c>
+      <c r="D3" s="3">
+        <v>39769</v>
       </c>
       <c r="E3">
         <v>122</v>
@@ -779,19 +735,19 @@
         <v>141</v>
       </c>
       <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L3" s="2">
         <v>44620</v>
@@ -808,17 +764,17 @@
       <c r="P3" s="2">
         <v>46263</v>
       </c>
-      <c r="Q3" t="s">
-        <v>50</v>
+      <c r="Q3">
+        <v>575.01</v>
       </c>
       <c r="R3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S3" s="2">
         <v>44812</v>
       </c>
-      <c r="T3" t="s">
-        <v>54</v>
+      <c r="T3">
+        <v>75.010000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -826,13 +782,13 @@
         <v>395</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="4">
-        <v>41.254542117055145</v>
+        <v>33</v>
+      </c>
+      <c r="D4" s="3">
+        <v>41254</v>
       </c>
       <c r="E4">
         <v>134</v>
@@ -844,16 +800,16 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" t="s">
-        <v>41</v>
-      </c>
       <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
         <v>44</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
       </c>
       <c r="L4" s="2">
         <v>44621</v>
@@ -870,17 +826,17 @@
       <c r="P4" s="2">
         <v>46264</v>
       </c>
-      <c r="Q4" t="s">
-        <v>51</v>
+      <c r="Q4">
+        <v>575.02</v>
       </c>
       <c r="R4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S4" s="2">
         <v>44813</v>
       </c>
-      <c r="T4" t="s">
-        <v>55</v>
+      <c r="T4">
+        <v>75.02</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -888,13 +844,13 @@
         <v>3165</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4">
-        <v>47.749099195226599</v>
+        <v>34</v>
+      </c>
+      <c r="D5" s="3">
+        <v>47749</v>
       </c>
       <c r="E5">
         <v>140</v>
@@ -909,13 +865,13 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L5" s="2">
         <v>44622</v>
@@ -932,17 +888,17 @@
       <c r="P5" s="2">
         <v>46265</v>
       </c>
-      <c r="Q5" t="s">
-        <v>52</v>
+      <c r="Q5">
+        <v>575.03</v>
       </c>
       <c r="R5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S5" s="2">
         <v>44814</v>
       </c>
-      <c r="T5" t="s">
-        <v>56</v>
+      <c r="T5">
+        <v>75.03</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -950,13 +906,13 @@
         <v>174058</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="4">
-        <v>42.83529966431815</v>
+        <v>35</v>
+      </c>
+      <c r="D6" s="3">
+        <v>42835</v>
       </c>
       <c r="E6">
         <v>125</v>
@@ -965,19 +921,19 @@
         <v>126</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L6" s="2">
         <v>44623</v>
@@ -994,17 +950,17 @@
       <c r="P6" s="2">
         <v>46266</v>
       </c>
-      <c r="Q6" t="s">
-        <v>53</v>
+      <c r="Q6">
+        <v>575.04</v>
       </c>
       <c r="R6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S6" s="2">
         <v>44815</v>
       </c>
-      <c r="T6" t="s">
-        <v>57</v>
+      <c r="T6">
+        <v>75.040000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REST API set up
</commit_message>
<xml_diff>
--- a/src/main/resources/hr-leaseplan.xlsx
+++ b/src/main/resources/hr-leaseplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eclipse-workspace\hr-leaseplan-project\hr-leaseplan-project\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE28BC5-054A-478F-A46E-155CCDB4CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0DD216-FC3E-4D3B-824D-9B5A6AC7389D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3720" windowWidth="29040" windowHeight="15840" xr2:uid="{7F8BE8A6-5FEF-41F6-9968-76C7035C40E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7F8BE8A6-5FEF-41F6-9968-76C7035C40E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Employee Number</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Nguyen, Khanh-Michel</t>
-  </si>
-  <si>
-    <t>Wick, John</t>
   </si>
   <si>
     <t>Belcaid, Younes</t>
@@ -563,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418E76DB-9A9E-421F-B9A7-2282E37ED3C7}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +720,7 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3">
         <v>39769</v>
@@ -735,19 +732,19 @@
         <v>141</v>
       </c>
       <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L3" s="2">
         <v>44620</v>
@@ -785,7 +782,7 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3">
         <v>41254</v>
@@ -800,16 +797,16 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4" s="2">
         <v>44621</v>
@@ -841,13 +838,13 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3165</v>
+        <v>53331</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3">
         <v>47749</v>
@@ -865,13 +862,13 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L5" s="2">
         <v>44622</v>
@@ -906,10 +903,10 @@
         <v>174058</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3">
         <v>42835</v>
@@ -921,19 +918,19 @@
         <v>126</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L6" s="2">
         <v>44623</v>

</xml_diff>